<commit_message>
Update table of reads per taxa
</commit_message>
<xml_diff>
--- a/sequences_processing/ITS2_CLC/ITS2_phylum_reads.xlsx
+++ b/sequences_processing/ITS2_CLC/ITS2_phylum_reads.xlsx
@@ -527,10 +527,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>20587</v>
+        <v>20535</v>
       </c>
       <c r="C2" t="n">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -539,13 +539,13 @@
         <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>12634</v>
+        <v>12683</v>
       </c>
     </row>
     <row r="3">
@@ -553,25 +553,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>23336</v>
+        <v>23389</v>
       </c>
       <c r="C3" t="n">
-        <v>340</v>
+        <v>322</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>9695</v>
+        <v>9661</v>
       </c>
     </row>
     <row r="4">
@@ -579,25 +579,25 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>24751</v>
+        <v>24813</v>
       </c>
       <c r="C4" t="n">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>8504</v>
+        <v>8436</v>
       </c>
     </row>
     <row r="5">
@@ -605,25 +605,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>24175</v>
+        <v>24229</v>
       </c>
       <c r="C5" t="n">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>8708</v>
+        <v>8666</v>
       </c>
     </row>
     <row r="6">
@@ -631,25 +631,25 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>22259</v>
+        <v>22092</v>
       </c>
       <c r="C6" t="n">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>10968</v>
+        <v>11164</v>
       </c>
     </row>
     <row r="7">
@@ -657,10 +657,10 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>24088</v>
+        <v>24012</v>
       </c>
       <c r="C7" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -669,13 +669,13 @@
         <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>9218</v>
+        <v>9299</v>
       </c>
     </row>
     <row r="8">
@@ -683,10 +683,10 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>26553</v>
+        <v>26612</v>
       </c>
       <c r="C8" t="n">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
@@ -695,13 +695,13 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>6748</v>
+        <v>6678</v>
       </c>
     </row>
     <row r="9">
@@ -709,7 +709,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>24599</v>
+        <v>24606</v>
       </c>
       <c r="C9" t="n">
         <v>54</v>
@@ -721,13 +721,13 @@
         <v>3</v>
       </c>
       <c r="F9" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>8733</v>
+        <v>8723</v>
       </c>
     </row>
     <row r="10">
@@ -735,25 +735,25 @@
         <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>25121</v>
+        <v>25108</v>
       </c>
       <c r="C10" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>8214</v>
+        <v>8223</v>
       </c>
     </row>
     <row r="11">
@@ -761,16 +761,16 @@
         <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>24876</v>
+        <v>24875</v>
       </c>
       <c r="C11" t="n">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>6</v>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>8311</v>
+        <v>8290</v>
       </c>
     </row>
     <row r="12">
@@ -787,16 +787,16 @@
         <v>18</v>
       </c>
       <c r="B12" t="n">
-        <v>25889</v>
+        <v>25964</v>
       </c>
       <c r="C12" t="n">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -805,7 +805,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>7296</v>
+        <v>7231</v>
       </c>
     </row>
     <row r="13">
@@ -813,25 +813,25 @@
         <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>22444</v>
+        <v>22434</v>
       </c>
       <c r="C13" t="n">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>10682</v>
+        <v>10686</v>
       </c>
     </row>
     <row r="14">
@@ -839,10 +839,10 @@
         <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>22977</v>
+        <v>22962</v>
       </c>
       <c r="C14" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -851,13 +851,13 @@
         <v>7</v>
       </c>
       <c r="F14" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>10312</v>
+        <v>10315</v>
       </c>
     </row>
     <row r="15">
@@ -865,25 +865,25 @@
         <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>24872</v>
+        <v>24938</v>
       </c>
       <c r="C15" t="n">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>8398</v>
+        <v>8349</v>
       </c>
     </row>
     <row r="16">
@@ -891,16 +891,16 @@
         <v>22</v>
       </c>
       <c r="B16" t="n">
-        <v>21503</v>
+        <v>21475</v>
       </c>
       <c r="C16" t="n">
         <v>139</v>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>3</v>
@@ -909,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>11755</v>
+        <v>11786</v>
       </c>
     </row>
     <row r="17">
@@ -917,25 +917,25 @@
         <v>23</v>
       </c>
       <c r="B17" t="n">
-        <v>27547</v>
+        <v>27596</v>
       </c>
       <c r="C17" t="n">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>5565</v>
+        <v>5518</v>
       </c>
     </row>
     <row r="18">
@@ -943,10 +943,10 @@
         <v>24</v>
       </c>
       <c r="B18" t="n">
-        <v>27133</v>
+        <v>27038</v>
       </c>
       <c r="C18" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -961,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>6165</v>
+        <v>6264</v>
       </c>
     </row>
     <row r="19">
@@ -969,25 +969,25 @@
         <v>25</v>
       </c>
       <c r="B19" t="n">
-        <v>22444</v>
+        <v>22392</v>
       </c>
       <c r="C19" t="n">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>10683</v>
+        <v>10734</v>
       </c>
     </row>
     <row r="20">
@@ -995,25 +995,25 @@
         <v>26</v>
       </c>
       <c r="B20" t="n">
-        <v>26794</v>
+        <v>26824</v>
       </c>
       <c r="C20" t="n">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D20" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>6180</v>
+        <v>6154</v>
       </c>
     </row>
     <row r="21">
@@ -1021,25 +1021,25 @@
         <v>27</v>
       </c>
       <c r="B21" t="n">
-        <v>23950</v>
+        <v>24065</v>
       </c>
       <c r="C21" t="n">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>9167</v>
+        <v>9061</v>
       </c>
     </row>
     <row r="22">
@@ -1047,10 +1047,10 @@
         <v>28</v>
       </c>
       <c r="B22" t="n">
-        <v>25525</v>
+        <v>25571</v>
       </c>
       <c r="C22" t="n">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -1059,13 +1059,13 @@
         <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>7522</v>
+        <v>7488</v>
       </c>
     </row>
     <row r="23">
@@ -1073,7 +1073,7 @@
         <v>29</v>
       </c>
       <c r="B23" t="n">
-        <v>23766</v>
+        <v>23767</v>
       </c>
       <c r="C23" t="n">
         <v>134</v>
@@ -1091,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>9496</v>
+        <v>9500</v>
       </c>
     </row>
     <row r="24">
@@ -1099,10 +1099,10 @@
         <v>30</v>
       </c>
       <c r="B24" t="n">
-        <v>23061</v>
+        <v>23112</v>
       </c>
       <c r="C24" t="n">
-        <v>695</v>
+        <v>706</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1111,13 +1111,13 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>9622</v>
+        <v>9559</v>
       </c>
     </row>
     <row r="25">
@@ -1125,25 +1125,25 @@
         <v>31</v>
       </c>
       <c r="B25" t="n">
-        <v>25875</v>
+        <v>25833</v>
       </c>
       <c r="C25" t="n">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>7316</v>
+        <v>7360</v>
       </c>
     </row>
     <row r="26">
@@ -1151,10 +1151,10 @@
         <v>32</v>
       </c>
       <c r="B26" t="n">
-        <v>12690</v>
+        <v>12734</v>
       </c>
       <c r="C26" t="n">
-        <v>337</v>
+        <v>349</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1163,13 +1163,13 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>20348</v>
+        <v>20296</v>
       </c>
     </row>
     <row r="27">
@@ -1177,25 +1177,25 @@
         <v>33</v>
       </c>
       <c r="B27" t="n">
-        <v>24724</v>
+        <v>24638</v>
       </c>
       <c r="C27" t="n">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>8331</v>
+        <v>8419</v>
       </c>
     </row>
     <row r="28">
@@ -1203,25 +1203,25 @@
         <v>34</v>
       </c>
       <c r="B28" t="n">
-        <v>24330</v>
+        <v>24406</v>
       </c>
       <c r="C28" t="n">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>8929</v>
+        <v>8877</v>
       </c>
     </row>
     <row r="29">
@@ -1229,16 +1229,16 @@
         <v>35</v>
       </c>
       <c r="B29" t="n">
-        <v>26642</v>
+        <v>26677</v>
       </c>
       <c r="C29" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -1247,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>6662</v>
+        <v>6622</v>
       </c>
     </row>
     <row r="30">
@@ -1255,25 +1255,25 @@
         <v>36</v>
       </c>
       <c r="B30" t="n">
-        <v>27186</v>
+        <v>27174</v>
       </c>
       <c r="C30" t="n">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>6119</v>
+        <v>6136</v>
       </c>
     </row>
     <row r="31">
@@ -1281,7 +1281,7 @@
         <v>37</v>
       </c>
       <c r="B31" t="n">
-        <v>21066</v>
+        <v>21065</v>
       </c>
       <c r="C31" t="n">
         <v>334</v>
@@ -1299,7 +1299,7 @@
         <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>11940</v>
+        <v>11943</v>
       </c>
     </row>
     <row r="32">
@@ -1307,25 +1307,25 @@
         <v>38</v>
       </c>
       <c r="B32" t="n">
-        <v>20893</v>
+        <v>20911</v>
       </c>
       <c r="C32" t="n">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>12372</v>
+        <v>12334</v>
       </c>
     </row>
     <row r="33">
@@ -1333,25 +1333,25 @@
         <v>39</v>
       </c>
       <c r="B33" t="n">
-        <v>25838</v>
+        <v>25908</v>
       </c>
       <c r="C33" t="n">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
+        <v>5</v>
+      </c>
+      <c r="F33" t="n">
         <v>3</v>
       </c>
-      <c r="F33" t="n">
-        <v>4</v>
-      </c>
       <c r="G33" t="n">
         <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>7418</v>
+        <v>7331</v>
       </c>
     </row>
     <row r="34">
@@ -1359,25 +1359,25 @@
         <v>40</v>
       </c>
       <c r="B34" t="n">
-        <v>25251</v>
+        <v>25203</v>
       </c>
       <c r="C34" t="n">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>7768</v>
+        <v>7842</v>
       </c>
     </row>
     <row r="35">
@@ -1385,25 +1385,25 @@
         <v>41</v>
       </c>
       <c r="B35" t="n">
-        <v>25396</v>
+        <v>25340</v>
       </c>
       <c r="C35" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>7936</v>
+        <v>7994</v>
       </c>
     </row>
     <row r="36">
@@ -1411,25 +1411,25 @@
         <v>42</v>
       </c>
       <c r="B36" t="n">
-        <v>27676</v>
+        <v>27702</v>
       </c>
       <c r="C36" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>5674</v>
+        <v>5654</v>
       </c>
     </row>
     <row r="37">
@@ -1437,10 +1437,10 @@
         <v>43</v>
       </c>
       <c r="B37" t="n">
-        <v>27135</v>
+        <v>27143</v>
       </c>
       <c r="C37" t="n">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
@@ -1455,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>6130</v>
+        <v>6137</v>
       </c>
     </row>
     <row r="38">
@@ -1463,25 +1463,25 @@
         <v>44</v>
       </c>
       <c r="B38" t="n">
-        <v>25341</v>
+        <v>25509</v>
       </c>
       <c r="C38" t="n">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D38" t="n">
         <v>1</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>8013</v>
+        <v>7859</v>
       </c>
     </row>
     <row r="39">
@@ -1489,10 +1489,10 @@
         <v>45</v>
       </c>
       <c r="B39" t="n">
-        <v>27567</v>
+        <v>27590</v>
       </c>
       <c r="C39" t="n">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -1501,13 +1501,13 @@
         <v>1</v>
       </c>
       <c r="F39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G39" t="n">
         <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>5576</v>
+        <v>5564</v>
       </c>
     </row>
     <row r="40">
@@ -1515,25 +1515,25 @@
         <v>46</v>
       </c>
       <c r="B40" t="n">
-        <v>27558</v>
+        <v>27498</v>
       </c>
       <c r="C40" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G40" t="n">
         <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>5702</v>
+        <v>5761</v>
       </c>
     </row>
     <row r="41">
@@ -1541,10 +1541,10 @@
         <v>47</v>
       </c>
       <c r="B41" t="n">
-        <v>27344</v>
+        <v>27243</v>
       </c>
       <c r="C41" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
@@ -1553,13 +1553,13 @@
         <v>2</v>
       </c>
       <c r="F41" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G41" t="n">
         <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>5978</v>
+        <v>6077</v>
       </c>
     </row>
     <row r="42">
@@ -1567,25 +1567,25 @@
         <v>48</v>
       </c>
       <c r="B42" t="n">
-        <v>27758</v>
+        <v>27666</v>
       </c>
       <c r="C42" t="n">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D42" t="n">
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G42" t="n">
         <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>5548</v>
+        <v>5650</v>
       </c>
     </row>
     <row r="43">
@@ -1593,25 +1593,25 @@
         <v>49</v>
       </c>
       <c r="B43" t="n">
-        <v>25078</v>
+        <v>25301</v>
       </c>
       <c r="C43" t="n">
-        <v>714</v>
+        <v>639</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>7600</v>
+        <v>7456</v>
       </c>
     </row>
     <row r="44">
@@ -1619,25 +1619,25 @@
         <v>50</v>
       </c>
       <c r="B44" t="n">
-        <v>28475</v>
+        <v>28462</v>
       </c>
       <c r="C44" t="n">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>4869</v>
+        <v>4895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>